<commit_message>
New reader - Anastasia
</commit_message>
<xml_diff>
--- a/Ion.xlsx
+++ b/Ion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>№</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Luceafărul</t>
+  </si>
+  <si>
+    <t>Артуром Конаном Дойлом</t>
+  </si>
+  <si>
+    <t>Шерлок холмс</t>
   </si>
 </sst>
 </file>
@@ -41,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,10 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -392,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +441,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44492</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ion card - new registry (Turgenev)
</commit_message>
<xml_diff>
--- a/Ion.xlsx
+++ b/Ion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>№</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>стр. 1</t>
+  </si>
+  <si>
+    <t>И.С. Тургенев</t>
+  </si>
+  <si>
+    <t>Отцы и дети</t>
+  </si>
+  <si>
+    <t>стр.45</t>
   </si>
 </sst>
 </file>
@@ -67,12 +76,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -102,12 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -409,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,19 +442,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -473,6 +490,23 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44498</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>